<commit_message>
New Telegram Bot Version
Perubahan : Merubah library bot telegram karena error akibat missmatch versi python dan urlib3
To do : Menugbah semua function menjadi async dan menambahkan await pada context.bot,sendMessage
</commit_message>
<xml_diff>
--- a/data/log/log.xlsx
+++ b/data/log/log.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F22" sqref="F22:G22"/>
@@ -2115,6 +2115,24 @@
         </is>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>2024-06-23 21:21:06.413886</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pembuatan download tambah daya EIS
Sudah : Sampai load menu pelayanan
TO do : Menunggu sampai excelnya terdownload
</commit_message>
<xml_diff>
--- a/data/log/log.xlsx
+++ b/data/log/log.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F22" sqref="F22:G22"/>
@@ -2133,6 +2133,24 @@
         </is>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>2024-06-24 19:16:51.358957</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Berhasil update laporan TS dan PD harian
Berhasil :
1. Update laporan TS Otomatis setiap jam 18.00
2. Berhasil buat script untuk request kirim laporan manual
3. Berhasil update laporan Penetapan P1 dan PD H-1 setiap jam 20.00

To do :
1. Buat script tambahan untuk log history fungsi update PD dan JN max
</commit_message>
<xml_diff>
--- a/data/log/log.xlsx
+++ b/data/log/log.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D168"/>
+  <dimension ref="A1:D263"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F22" sqref="F22:G22"/>
@@ -3465,6 +3465,1716 @@
         </is>
       </c>
     </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>168</v>
+      </c>
+      <c r="B169" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>2024-07-12 16:59:45.223620</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>169</v>
+      </c>
+      <c r="B170" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:00:28.454365</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>170</v>
+      </c>
+      <c r="B171" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:01:23.535991</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>171</v>
+      </c>
+      <c r="B172" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:02:45.069265</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>172</v>
+      </c>
+      <c r="B173" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:03:21.986726</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:08:36.975343</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>174</v>
+      </c>
+      <c r="B175" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:49:23.977072</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>175</v>
+      </c>
+      <c r="B176" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:50:06.990008</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>176</v>
+      </c>
+      <c r="B177" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:50:48.640268</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>177</v>
+      </c>
+      <c r="B178" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:51:38.113849</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>178</v>
+      </c>
+      <c r="B179" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:52:12.426666</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>179</v>
+      </c>
+      <c r="B180" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:52:46.408425</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>180</v>
+      </c>
+      <c r="B181" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:57:02.321051</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>181</v>
+      </c>
+      <c r="B182" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:57:36.748340</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>182</v>
+      </c>
+      <c r="B183" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>2024-07-12 17:58:13.293826</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>183</v>
+      </c>
+      <c r="B184" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>2024-07-12 18:17:13.060038</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>184</v>
+      </c>
+      <c r="B185" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>2024-07-12 18:20:43.623502</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>185</v>
+      </c>
+      <c r="B186" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>2024-07-12 18:48:01.302773</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>186</v>
+      </c>
+      <c r="B187" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>2024-07-12 19:36:24.980040</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>187</v>
+      </c>
+      <c r="B188" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>2024-07-12 19:37:01.820898</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>188</v>
+      </c>
+      <c r="B189" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>2024-07-15 18:33:58.056896</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>189</v>
+      </c>
+      <c r="B190" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>2024-07-15 18:34:26.881198</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>190</v>
+      </c>
+      <c r="B191" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>2024-07-16 16:18:58.346956</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>191</v>
+      </c>
+      <c r="B192" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>2024-07-16 16:20:01.036335</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>192</v>
+      </c>
+      <c r="B193" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>2024-07-16 16:20:15.053284</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>193</v>
+      </c>
+      <c r="B194" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>2024-07-16 16:22:36.458810</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>194</v>
+      </c>
+      <c r="B195" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>2024-07-16 17:18:53.376448</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>195</v>
+      </c>
+      <c r="B196" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>2024-07-16 17:22:59.858737</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>196</v>
+      </c>
+      <c r="B197" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>2024-07-16 17:23:56.964588</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>197</v>
+      </c>
+      <c r="B198" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>2024-07-16 17:43:45.428532</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>198</v>
+      </c>
+      <c r="B199" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>2024-07-16 17:47:33.290038</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>199</v>
+      </c>
+      <c r="B200" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>2024-07-16 17:51:19.894328</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>200</v>
+      </c>
+      <c r="B201" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>2024-07-16 17:51:47.536472</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>201</v>
+      </c>
+      <c r="B202" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>2024-07-16 18:20:58.190255</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>202</v>
+      </c>
+      <c r="B203" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>2024-07-16 18:30:47.007821</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>203</v>
+      </c>
+      <c r="B204" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>2024-07-16 18:34:35.970999</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>204</v>
+      </c>
+      <c r="B205" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>2024-07-16 18:43:04.730593</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>205</v>
+      </c>
+      <c r="B206" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>2024-07-17 16:48:33.144739</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>206</v>
+      </c>
+      <c r="B207" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>2024-07-17 16:49:44.722156</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>207</v>
+      </c>
+      <c r="B208" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>2024-07-17 16:55:58.469196</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>208</v>
+      </c>
+      <c r="B209" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>2024-07-17 16:57:22.832740</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>209</v>
+      </c>
+      <c r="B210" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>2024-07-17 18:06:41.224621</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>210</v>
+      </c>
+      <c r="B211" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>2024-07-17 18:31:34.236716</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>211</v>
+      </c>
+      <c r="B212" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>2024-07-17 18:34:06.876737</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>212</v>
+      </c>
+      <c r="B213" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>2024-07-17 19:02:18.587324</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>213</v>
+      </c>
+      <c r="B214" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>2024-07-17 19:02:46.785627</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>214</v>
+      </c>
+      <c r="B215" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Infoblokir</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>2024-07-17 19:05:04.646312</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>215</v>
+      </c>
+      <c r="B216" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>2024-07-17 19:28:14.301688</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>216</v>
+      </c>
+      <c r="B217" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>2024-07-17 19:35:16.431070</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>217</v>
+      </c>
+      <c r="B218" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>2024-07-18 16:42:54.753470</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>218</v>
+      </c>
+      <c r="B219" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>2024-07-18 18:55:08.902888</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>219</v>
+      </c>
+      <c r="B220" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>2024-07-18 19:13:14.771659</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>220</v>
+      </c>
+      <c r="B221" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>2024-07-18 19:14:01.789270</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>221</v>
+      </c>
+      <c r="B222" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>2024-07-19 17:35:18.319056</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>222</v>
+      </c>
+      <c r="B223" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>2024-07-19 17:47:55.907440</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>223</v>
+      </c>
+      <c r="B224" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>2024-07-19 17:57:49.958640</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>224</v>
+      </c>
+      <c r="B225" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>2024-07-19 18:53:40.176334</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>225</v>
+      </c>
+      <c r="B226" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>2024-07-19 18:57:08.851350</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>226</v>
+      </c>
+      <c r="B227" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>2024-07-19 18:57:32.461673</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>227</v>
+      </c>
+      <c r="B228" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>2024-07-19 20:20:58.633929</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>228</v>
+      </c>
+      <c r="B229" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>2024-07-21 10:17:40.413288</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>229</v>
+      </c>
+      <c r="B230" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>2024-07-21 13:57:58.185753</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>230</v>
+      </c>
+      <c r="B231" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>2024-07-22 15:05:33.583567</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>231</v>
+      </c>
+      <c r="B232" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>2024-07-22 16:27:30.496507</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>232</v>
+      </c>
+      <c r="B233" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>2024-07-22 17:37:53.692642</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>233</v>
+      </c>
+      <c r="B234" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>2024-07-22 17:38:48.437114</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>234</v>
+      </c>
+      <c r="B235" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>2024-07-22 18:42:06.144046</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>235</v>
+      </c>
+      <c r="B236" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>2024-07-22 18:48:02.131867</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>236</v>
+      </c>
+      <c r="B237" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>2024-07-22 18:52:08.787718</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>237</v>
+      </c>
+      <c r="B238" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>2024-07-22 19:07:38.503144</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>238</v>
+      </c>
+      <c r="B239" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>2024-07-22 19:16:57.353659</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>239</v>
+      </c>
+      <c r="B240" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>2024-07-23 18:50:05.814244</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>240</v>
+      </c>
+      <c r="B241" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>2024-07-23 19:07:55.391653</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>241</v>
+      </c>
+      <c r="B242" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>2024-07-23 19:08:40.984100</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>242</v>
+      </c>
+      <c r="B243" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>2024-07-23 19:24:54.170897</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>243</v>
+      </c>
+      <c r="B244" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>2024-07-23 19:30:01.344552</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>244</v>
+      </c>
+      <c r="B245" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>2024-07-23 19:39:43.045547</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>245</v>
+      </c>
+      <c r="B246" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>2024-07-23 19:55:37.009471</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>246</v>
+      </c>
+      <c r="B247" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>2024-07-23 20:13:12.088714</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>247</v>
+      </c>
+      <c r="B248" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>2024-07-24 16:24:34.415205</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>248</v>
+      </c>
+      <c r="B249" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>2024-07-24 18:49:39.199493</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>249</v>
+      </c>
+      <c r="B250" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>2024-07-24 18:56:16.431415</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>250</v>
+      </c>
+      <c r="B251" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>2024-07-25 16:44:37.739633</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>251</v>
+      </c>
+      <c r="B252" t="n">
+        <v>6473262382</v>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>2024-07-25 16:45:41.334184</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>252</v>
+      </c>
+      <c r="B253" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>2024-07-25 16:54:34.900448</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>253</v>
+      </c>
+      <c r="B254" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>2024-07-25 20:05:38.175271</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>254</v>
+      </c>
+      <c r="B255" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>2024-07-25 20:12:59.564367</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>255</v>
+      </c>
+      <c r="B256" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>2024-07-25 20:13:29.669824</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>256</v>
+      </c>
+      <c r="B257" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>2024-07-25 20:37:55.458468</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>257</v>
+      </c>
+      <c r="B258" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>2024-07-25 20:41:28.944838</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>258</v>
+      </c>
+      <c r="B259" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>2024-07-25 20:42:01.247510</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>259</v>
+      </c>
+      <c r="B260" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>2024-07-25 20:44:00.271809</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>260</v>
+      </c>
+      <c r="B261" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>2024-07-26 18:03:37.725262</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>261</v>
+      </c>
+      <c r="B262" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>2024-07-26 18:04:11.118060</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>262</v>
+      </c>
+      <c r="B263" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>2024-07-26 18:07:51.409143</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update laporan jn max ke uid
Mengkondisikan jika update berhasil,, mengupdate ke spreadsheet UID
menghapus auto send report ke wa uid
</commit_message>
<xml_diff>
--- a/data/log/log.xlsx
+++ b/data/log/log.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D425"/>
+  <dimension ref="A1:D628"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F22" sqref="F22:G22"/>
@@ -8091,6 +8091,3660 @@
         </is>
       </c>
     </row>
+    <row r="426">
+      <c r="A426" t="n">
+        <v>425</v>
+      </c>
+      <c r="B426" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>2024-08-24 15:46:28.758678</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="n">
+        <v>426</v>
+      </c>
+      <c r="B427" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>2024-08-25 08:43:00.936511</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="n">
+        <v>427</v>
+      </c>
+      <c r="B428" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>2024-08-25 08:47:30.789512</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="n">
+        <v>428</v>
+      </c>
+      <c r="B429" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>2024-08-25 08:48:13.469298</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="n">
+        <v>429</v>
+      </c>
+      <c r="B430" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>2024-08-25 08:55:12.513280</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="n">
+        <v>430</v>
+      </c>
+      <c r="B431" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>2024-08-25 09:02:23.094076</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="n">
+        <v>431</v>
+      </c>
+      <c r="B432" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>2024-08-25 09:13:27.876064</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="n">
+        <v>432</v>
+      </c>
+      <c r="B433" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>2024-08-25 18:05:43.748893</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="n">
+        <v>433</v>
+      </c>
+      <c r="B434" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>Mengirim Laporan Realisasi Tindak Lanjut JN Max Otomatis</t>
+        </is>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>2024-08-25 19:02:49.608886</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="n">
+        <v>434</v>
+      </c>
+      <c r="B435" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Otomatis</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>2024-08-25 20:00:32.522154</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="n">
+        <v>435</v>
+      </c>
+      <c r="B436" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>2024-08-25 20:31:52.881516</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="n">
+        <v>436</v>
+      </c>
+      <c r="B437" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>2024-08-25 21:21:13.408557</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="n">
+        <v>437</v>
+      </c>
+      <c r="B438" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>2024-08-26 10:48:00.336736</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="n">
+        <v>438</v>
+      </c>
+      <c r="B439" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>2024-08-26 11:09:40.569012</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="n">
+        <v>439</v>
+      </c>
+      <c r="B440" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>2024-08-26 13:05:53.231298</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="n">
+        <v>440</v>
+      </c>
+      <c r="B441" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>2024-08-26 16:30:23.776930</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="n">
+        <v>441</v>
+      </c>
+      <c r="B442" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>2024-08-26 16:30:45.012971</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="n">
+        <v>442</v>
+      </c>
+      <c r="B443" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>2024-08-26 16:31:18.346953</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="n">
+        <v>443</v>
+      </c>
+      <c r="B444" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>2024-08-26 16:36:40.169119</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="n">
+        <v>444</v>
+      </c>
+      <c r="B445" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>2024-08-26 16:43:08.512422</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="n">
+        <v>445</v>
+      </c>
+      <c r="B446" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>2024-08-26 16:43:27.317933</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="n">
+        <v>446</v>
+      </c>
+      <c r="B447" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>2024-08-26 16:50:51.908395</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="n">
+        <v>447</v>
+      </c>
+      <c r="B448" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>2024-08-26 16:53:47.437648</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="n">
+        <v>448</v>
+      </c>
+      <c r="B449" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>2024-08-26 18:05:04.644972</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="n">
+        <v>449</v>
+      </c>
+      <c r="B450" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>Mengirim Laporan Realisasi Tindak Lanjut JN Max Otomatis</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>2024-08-26 19:01:09.896097</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="n">
+        <v>450</v>
+      </c>
+      <c r="B451" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>2024-08-26 19:18:18.706862</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="n">
+        <v>451</v>
+      </c>
+      <c r="B452" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>Mengirim Laporan Realisasi Tindak Lanjut JN Max Manual</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>2024-08-26 19:20:02.551071</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="n">
+        <v>452</v>
+      </c>
+      <c r="B453" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>Mengirim Laporan Realisasi Tindak Lanjut JN Max Manual</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>2024-08-26 19:33:46.149550</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="n">
+        <v>453</v>
+      </c>
+      <c r="B454" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>2024-08-26 19:46:21.374791</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="n">
+        <v>454</v>
+      </c>
+      <c r="B455" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>2024-08-26 19:47:03.046262</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="n">
+        <v>455</v>
+      </c>
+      <c r="B456" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Otomatis</t>
+        </is>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>2024-08-26 20:00:38.225469</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="n">
+        <v>456</v>
+      </c>
+      <c r="B457" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>2024-08-26 20:36:18.782328</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="n">
+        <v>457</v>
+      </c>
+      <c r="B458" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>2024-08-27 13:24:48.542208</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="n">
+        <v>458</v>
+      </c>
+      <c r="B459" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>2024-08-27 13:28:53.964453</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="n">
+        <v>459</v>
+      </c>
+      <c r="B460" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>2024-08-27 13:29:12.460539</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="n">
+        <v>460</v>
+      </c>
+      <c r="B461" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:19:06.964179</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="n">
+        <v>461</v>
+      </c>
+      <c r="B462" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:19:53.023557</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="n">
+        <v>462</v>
+      </c>
+      <c r="B463" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>2024-08-27 16:44:24.504989</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="n">
+        <v>463</v>
+      </c>
+      <c r="B464" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>2024-08-27 16:45:29.497115</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="n">
+        <v>464</v>
+      </c>
+      <c r="B465" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D465" t="inlineStr">
+        <is>
+          <t>2024-08-27 16:59:09.408768</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="n">
+        <v>465</v>
+      </c>
+      <c r="B466" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>2024-08-27 17:33:42.091708</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="n">
+        <v>466</v>
+      </c>
+      <c r="B467" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>Mengirim Laporan Realisasi Tindak Lanjut JN Max Otomatis</t>
+        </is>
+      </c>
+      <c r="D467" t="inlineStr">
+        <is>
+          <t>2024-08-27 19:01:08.971834</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="n">
+        <v>467</v>
+      </c>
+      <c r="B468" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>Mengirim Laporan Realisasi Tindak Lanjut JN Max Manual</t>
+        </is>
+      </c>
+      <c r="D468" t="inlineStr">
+        <is>
+          <t>2024-08-27 19:26:35.041564</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="n">
+        <v>468</v>
+      </c>
+      <c r="B469" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Otomatis</t>
+        </is>
+      </c>
+      <c r="D469" t="inlineStr">
+        <is>
+          <t>2024-08-27 20:00:33.807929</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="n">
+        <v>469</v>
+      </c>
+      <c r="B470" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D470" t="inlineStr">
+        <is>
+          <t>2024-08-27 20:32:00.265482</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="n">
+        <v>470</v>
+      </c>
+      <c r="B471" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D471" t="inlineStr">
+        <is>
+          <t>2024-08-28 11:14:00.851289</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="n">
+        <v>471</v>
+      </c>
+      <c r="B472" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D472" t="inlineStr">
+        <is>
+          <t>2024-08-28 11:19:33.691991</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="n">
+        <v>472</v>
+      </c>
+      <c r="B473" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D473" t="inlineStr">
+        <is>
+          <t>2024-08-28 11:24:46.388260</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="n">
+        <v>473</v>
+      </c>
+      <c r="B474" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D474" t="inlineStr">
+        <is>
+          <t>2024-08-28 11:25:11.845344</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="n">
+        <v>474</v>
+      </c>
+      <c r="B475" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>2024-08-28 16:36:37.823721</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="n">
+        <v>475</v>
+      </c>
+      <c r="B476" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D476" t="inlineStr">
+        <is>
+          <t>2024-08-28 16:40:40.989581</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="n">
+        <v>476</v>
+      </c>
+      <c r="B477" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>2024-08-28 16:46:05.773992</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="n">
+        <v>477</v>
+      </c>
+      <c r="B478" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D478" t="inlineStr">
+        <is>
+          <t>2024-08-28 16:46:27.984680</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="n">
+        <v>478</v>
+      </c>
+      <c r="B479" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D479" t="inlineStr">
+        <is>
+          <t>2024-08-28 16:46:46.568623</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="n">
+        <v>479</v>
+      </c>
+      <c r="B480" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D480" t="inlineStr">
+        <is>
+          <t>2024-08-28 18:08:05.544395</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="n">
+        <v>480</v>
+      </c>
+      <c r="B481" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D481" t="inlineStr">
+        <is>
+          <t>2024-08-28 18:55:14.054016</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="n">
+        <v>481</v>
+      </c>
+      <c r="B482" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>mengupdate laporan spreadsheet monitoring JN Max UID Manual</t>
+        </is>
+      </c>
+      <c r="D482" t="inlineStr">
+        <is>
+          <t>2024-08-28 19:04:51.346133</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="n">
+        <v>482</v>
+      </c>
+      <c r="B483" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D483" t="inlineStr">
+        <is>
+          <t>2024-08-28 20:33:52.155387</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="n">
+        <v>483</v>
+      </c>
+      <c r="B484" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D484" t="inlineStr">
+        <is>
+          <t>2024-08-29 14:40:19.695858</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="n">
+        <v>484</v>
+      </c>
+      <c r="B485" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D485" t="inlineStr">
+        <is>
+          <t>2024-08-29 14:41:04.497373</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="n">
+        <v>485</v>
+      </c>
+      <c r="B486" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>2024-08-29 15:41:23.771455</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="n">
+        <v>486</v>
+      </c>
+      <c r="B487" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>2024-08-29 15:41:55.962749</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="n">
+        <v>487</v>
+      </c>
+      <c r="B488" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>2024-08-29 16:20:06.462577</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="n">
+        <v>488</v>
+      </c>
+      <c r="B489" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>2024-08-29 16:27:37.222740</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="n">
+        <v>489</v>
+      </c>
+      <c r="B490" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>2024-08-29 16:48:13.115506</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="n">
+        <v>490</v>
+      </c>
+      <c r="B491" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>2024-08-29 17:39:32.053952</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="n">
+        <v>491</v>
+      </c>
+      <c r="B492" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>2024-08-29 17:40:00.477762</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="n">
+        <v>492</v>
+      </c>
+      <c r="B493" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>2024-08-29 18:08:12.623860</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="n">
+        <v>493</v>
+      </c>
+      <c r="B494" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>2024-08-29 19:07:29.950194</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="n">
+        <v>494</v>
+      </c>
+      <c r="B495" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>2024-08-29 19:08:07.499057</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="n">
+        <v>495</v>
+      </c>
+      <c r="B496" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>2024-08-29 20:31:52.855145</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="n">
+        <v>496</v>
+      </c>
+      <c r="B497" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>2024-08-30 05:46:42.108784</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="n">
+        <v>497</v>
+      </c>
+      <c r="B498" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>2024-08-30 05:47:04.801498</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="n">
+        <v>498</v>
+      </c>
+      <c r="B499" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>2024-08-30 13:53:55.817520</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="n">
+        <v>499</v>
+      </c>
+      <c r="B500" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>2024-08-30 13:55:32.579627</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="n">
+        <v>500</v>
+      </c>
+      <c r="B501" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>2024-08-30 14:57:54.125860</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="n">
+        <v>501</v>
+      </c>
+      <c r="B502" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>2024-08-30 14:58:17.796079</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="n">
+        <v>502</v>
+      </c>
+      <c r="B503" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>2024-08-30 15:31:05.774999</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="n">
+        <v>503</v>
+      </c>
+      <c r="B504" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>2024-08-30 15:31:30.508461</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="n">
+        <v>504</v>
+      </c>
+      <c r="B505" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>2024-08-30 16:33:17.042360</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="n">
+        <v>505</v>
+      </c>
+      <c r="B506" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>2024-08-30 16:33:40.003739</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="n">
+        <v>506</v>
+      </c>
+      <c r="B507" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>2024-08-30 16:38:40.869108</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="n">
+        <v>507</v>
+      </c>
+      <c r="B508" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:40:12.507646</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="n">
+        <v>508</v>
+      </c>
+      <c r="B509" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:20.402813</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="n">
+        <v>509</v>
+      </c>
+      <c r="B510" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:51:36.847859</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="n">
+        <v>510</v>
+      </c>
+      <c r="B511" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:55:28.956922</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="n">
+        <v>511</v>
+      </c>
+      <c r="B512" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:55:55.819621</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="n">
+        <v>512</v>
+      </c>
+      <c r="B513" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:56:13.309607</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="n">
+        <v>513</v>
+      </c>
+      <c r="B514" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>2024-08-30 18:04:20.382810</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="n">
+        <v>514</v>
+      </c>
+      <c r="B515" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>2024-08-30 20:35:08.507767</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="n">
+        <v>515</v>
+      </c>
+      <c r="B516" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>2024-08-30 21:17:56.910551</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="n">
+        <v>516</v>
+      </c>
+      <c r="B517" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D517" t="inlineStr">
+        <is>
+          <t>2024-08-30 21:21:51.953333</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="n">
+        <v>517</v>
+      </c>
+      <c r="B518" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D518" t="inlineStr">
+        <is>
+          <t>2024-08-30 21:22:11.168653</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="n">
+        <v>518</v>
+      </c>
+      <c r="B519" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>2024-08-30 21:31:47.763650</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="n">
+        <v>519</v>
+      </c>
+      <c r="B520" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D520" t="inlineStr">
+        <is>
+          <t>2024-08-31 18:04:40.793479</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="n">
+        <v>520</v>
+      </c>
+      <c r="B521" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D521" t="inlineStr">
+        <is>
+          <t>2024-08-31 20:34:22.152545</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="n">
+        <v>521</v>
+      </c>
+      <c r="B522" t="n">
+        <v>1029804860</v>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>2024-09-01 14:50:42.428465</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="n">
+        <v>522</v>
+      </c>
+      <c r="B523" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>2024-09-01 18:04:04.541572</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="n">
+        <v>523</v>
+      </c>
+      <c r="B524" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>2024-09-01 20:33:12.526554</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="n">
+        <v>524</v>
+      </c>
+      <c r="B525" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>2024-09-02 14:37:45.633680</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="n">
+        <v>525</v>
+      </c>
+      <c r="B526" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>2024-09-02 15:17:41.190614</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="n">
+        <v>526</v>
+      </c>
+      <c r="B527" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>2024-09-02 15:21:53.306985</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="n">
+        <v>527</v>
+      </c>
+      <c r="B528" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D528" t="inlineStr">
+        <is>
+          <t>2024-09-02 15:26:48.700369</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="n">
+        <v>528</v>
+      </c>
+      <c r="B529" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D529" t="inlineStr">
+        <is>
+          <t>2024-09-03 08:51:59.357703</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="n">
+        <v>529</v>
+      </c>
+      <c r="B530" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D530" t="inlineStr">
+        <is>
+          <t>2024-09-03 08:53:24.812496</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="n">
+        <v>530</v>
+      </c>
+      <c r="B531" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D531" t="inlineStr">
+        <is>
+          <t>2024-09-03 16:15:33.372316</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="n">
+        <v>531</v>
+      </c>
+      <c r="B532" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D532" t="inlineStr">
+        <is>
+          <t>2024-09-03 16:16:07.437509</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="n">
+        <v>532</v>
+      </c>
+      <c r="B533" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D533" t="inlineStr">
+        <is>
+          <t>2024-09-03 16:18:06.508330</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="n">
+        <v>533</v>
+      </c>
+      <c r="B534" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D534" t="inlineStr">
+        <is>
+          <t>2024-09-03 17:00:15.458312</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="n">
+        <v>534</v>
+      </c>
+      <c r="B535" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D535" t="inlineStr">
+        <is>
+          <t>2024-09-03 17:00:54.387214</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="n">
+        <v>535</v>
+      </c>
+      <c r="B536" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D536" t="inlineStr">
+        <is>
+          <t>2024-09-03 17:37:16.969776</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="n">
+        <v>536</v>
+      </c>
+      <c r="B537" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D537" t="inlineStr">
+        <is>
+          <t>2024-09-03 17:45:57.232055</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="n">
+        <v>537</v>
+      </c>
+      <c r="B538" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D538" t="inlineStr">
+        <is>
+          <t>2024-09-03 18:04:43.319138</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="n">
+        <v>538</v>
+      </c>
+      <c r="B539" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D539" t="inlineStr">
+        <is>
+          <t>2024-09-03 18:19:00.790843</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="n">
+        <v>539</v>
+      </c>
+      <c r="B540" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D540" t="inlineStr">
+        <is>
+          <t>2024-09-03 20:35:21.454735</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="n">
+        <v>540</v>
+      </c>
+      <c r="B541" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D541" t="inlineStr">
+        <is>
+          <t>2024-09-04 09:53:41.000559</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="n">
+        <v>541</v>
+      </c>
+      <c r="B542" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D542" t="inlineStr">
+        <is>
+          <t>2024-09-04 09:54:17.143235</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="n">
+        <v>542</v>
+      </c>
+      <c r="B543" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D543" t="inlineStr">
+        <is>
+          <t>2024-09-04 10:39:16.769880</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="n">
+        <v>543</v>
+      </c>
+      <c r="B544" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>2024-09-04 10:40:11.769645</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="n">
+        <v>544</v>
+      </c>
+      <c r="B545" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D545" t="inlineStr">
+        <is>
+          <t>2024-09-04 16:17:22.918753</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="n">
+        <v>545</v>
+      </c>
+      <c r="B546" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D546" t="inlineStr">
+        <is>
+          <t>2024-09-04 17:09:05.764920</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="n">
+        <v>546</v>
+      </c>
+      <c r="B547" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D547" t="inlineStr">
+        <is>
+          <t>2024-09-04 17:12:59.522845</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="n">
+        <v>547</v>
+      </c>
+      <c r="B548" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>2024-09-04 17:19:19.406863</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="n">
+        <v>548</v>
+      </c>
+      <c r="B549" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>2024-09-04 17:23:15.158733</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="n">
+        <v>549</v>
+      </c>
+      <c r="B550" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>2024-09-04 17:52:28.739142</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="n">
+        <v>550</v>
+      </c>
+      <c r="B551" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D551" t="inlineStr">
+        <is>
+          <t>2024-09-04 20:32:32.388525</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="n">
+        <v>551</v>
+      </c>
+      <c r="B552" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>Info Pelanggan</t>
+        </is>
+      </c>
+      <c r="D552" t="inlineStr">
+        <is>
+          <t>2024-09-05 12:25:58.756700</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="n">
+        <v>552</v>
+      </c>
+      <c r="B553" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>2024-09-05 14:59:20.869681</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="n">
+        <v>553</v>
+      </c>
+      <c r="B554" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D554" t="inlineStr">
+        <is>
+          <t>2024-09-05 15:00:25.038100</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="n">
+        <v>554</v>
+      </c>
+      <c r="B555" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D555" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:56:47.773250</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="n">
+        <v>555</v>
+      </c>
+      <c r="B556" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:57:58.877254</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="n">
+        <v>556</v>
+      </c>
+      <c r="B557" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D557" t="inlineStr">
+        <is>
+          <t>2024-09-05 17:31:52.563724</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="n">
+        <v>557</v>
+      </c>
+      <c r="B558" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>2024-09-05 17:35:30.331331</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="n">
+        <v>558</v>
+      </c>
+      <c r="B559" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D559" t="inlineStr">
+        <is>
+          <t>2024-09-05 18:03:58.894569</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="n">
+        <v>559</v>
+      </c>
+      <c r="B560" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D560" t="inlineStr">
+        <is>
+          <t>2024-09-05 20:31:56.443815</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="n">
+        <v>560</v>
+      </c>
+      <c r="B561" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D561" t="inlineStr">
+        <is>
+          <t>2024-09-06 08:49:36.541540</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="n">
+        <v>561</v>
+      </c>
+      <c r="B562" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D562" t="inlineStr">
+        <is>
+          <t>2024-09-06 10:09:41.468147</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="n">
+        <v>562</v>
+      </c>
+      <c r="B563" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D563" t="inlineStr">
+        <is>
+          <t>2024-09-06 10:12:10.787964</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="n">
+        <v>563</v>
+      </c>
+      <c r="B564" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D564" t="inlineStr">
+        <is>
+          <t>2024-09-06 14:37:43.150232</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="n">
+        <v>564</v>
+      </c>
+      <c r="B565" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>2024-09-06 15:09:02.475484</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="n">
+        <v>565</v>
+      </c>
+      <c r="B566" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>2024-09-06 15:12:50.718279</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="n">
+        <v>566</v>
+      </c>
+      <c r="B567" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D567" t="inlineStr">
+        <is>
+          <t>2024-09-06 15:21:17.258728</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="n">
+        <v>567</v>
+      </c>
+      <c r="B568" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>2024-09-06 15:21:42.143808</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="n">
+        <v>568</v>
+      </c>
+      <c r="B569" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>2024-09-06 15:22:05.430819</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="n">
+        <v>569</v>
+      </c>
+      <c r="B570" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>Mendowload Laporan TUL 309</t>
+        </is>
+      </c>
+      <c r="D570" t="inlineStr">
+        <is>
+          <t>2024-09-06 15:22:28.462515</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="n">
+        <v>570</v>
+      </c>
+      <c r="B571" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D571" t="inlineStr">
+        <is>
+          <t>2024-09-06 16:17:28.689635</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="n">
+        <v>571</v>
+      </c>
+      <c r="B572" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D572" t="inlineStr">
+        <is>
+          <t>2024-09-06 16:18:08.391071</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="n">
+        <v>572</v>
+      </c>
+      <c r="B573" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D573" t="inlineStr">
+        <is>
+          <t>2024-09-06 18:04:22.967563</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="n">
+        <v>573</v>
+      </c>
+      <c r="B574" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>2024-09-06 18:33:58.365479</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="n">
+        <v>574</v>
+      </c>
+      <c r="B575" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>2024-09-06 19:56:37.584620</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="n">
+        <v>575</v>
+      </c>
+      <c r="B576" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>2024-09-06 20:31:43.004584</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="n">
+        <v>576</v>
+      </c>
+      <c r="B577" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>2024-09-07 18:04:03.079007</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="n">
+        <v>577</v>
+      </c>
+      <c r="B578" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D578" t="inlineStr">
+        <is>
+          <t>2024-09-07 20:32:01.865214</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="n">
+        <v>578</v>
+      </c>
+      <c r="B579" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D579" t="inlineStr">
+        <is>
+          <t>2024-09-08 20:32:02.492410</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="n">
+        <v>579</v>
+      </c>
+      <c r="B580" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D580" t="inlineStr">
+        <is>
+          <t>2024-09-09 14:20:30.623239</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="n">
+        <v>580</v>
+      </c>
+      <c r="B581" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D581" t="inlineStr">
+        <is>
+          <t>2024-09-09 14:59:10.483374</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="n">
+        <v>581</v>
+      </c>
+      <c r="B582" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D582" t="inlineStr">
+        <is>
+          <t>2024-09-09 17:02:41.357060</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="n">
+        <v>582</v>
+      </c>
+      <c r="B583" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D583" t="inlineStr">
+        <is>
+          <t>2024-09-09 17:20:24.499033</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="n">
+        <v>583</v>
+      </c>
+      <c r="B584" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D584" t="inlineStr">
+        <is>
+          <t>2024-09-09 17:21:34.690770</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="n">
+        <v>584</v>
+      </c>
+      <c r="B585" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D585" t="inlineStr">
+        <is>
+          <t>2024-09-09 18:05:05.279935</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="n">
+        <v>585</v>
+      </c>
+      <c r="B586" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D586" t="inlineStr">
+        <is>
+          <t>2024-09-09 18:12:15.921494</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="n">
+        <v>586</v>
+      </c>
+      <c r="B587" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D587" t="inlineStr">
+        <is>
+          <t>2024-09-10 08:07:52.607141</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="n">
+        <v>587</v>
+      </c>
+      <c r="B588" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D588" t="inlineStr">
+        <is>
+          <t>2024-09-10 08:15:40.066930</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="n">
+        <v>588</v>
+      </c>
+      <c r="B589" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D589" t="inlineStr">
+        <is>
+          <t>2024-09-10 08:16:13.380782</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="n">
+        <v>589</v>
+      </c>
+      <c r="B590" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D590" t="inlineStr">
+        <is>
+          <t>2024-09-10 18:33:52.853745</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="n">
+        <v>590</v>
+      </c>
+      <c r="B591" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D591" t="inlineStr">
+        <is>
+          <t>2024-09-10 20:33:21.038284</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="n">
+        <v>591</v>
+      </c>
+      <c r="B592" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D592" t="inlineStr">
+        <is>
+          <t>2024-09-11 12:44:46.652803</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="n">
+        <v>592</v>
+      </c>
+      <c r="B593" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D593" t="inlineStr">
+        <is>
+          <t>2024-09-11 12:45:23.245138</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="n">
+        <v>593</v>
+      </c>
+      <c r="B594" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D594" t="inlineStr">
+        <is>
+          <t>2024-09-11 13:09:09.750547</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="n">
+        <v>594</v>
+      </c>
+      <c r="B595" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D595" t="inlineStr">
+        <is>
+          <t>2024-09-11 13:09:38.577319</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="n">
+        <v>595</v>
+      </c>
+      <c r="B596" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D596" t="inlineStr">
+        <is>
+          <t>2024-09-11 16:02:07.550679</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="n">
+        <v>596</v>
+      </c>
+      <c r="B597" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D597" t="inlineStr">
+        <is>
+          <t>2024-09-11 16:02:26.220254</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="n">
+        <v>597</v>
+      </c>
+      <c r="B598" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D598" t="inlineStr">
+        <is>
+          <t>2024-09-11 18:07:43.186874</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="n">
+        <v>598</v>
+      </c>
+      <c r="B599" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D599" t="inlineStr">
+        <is>
+          <t>2024-09-11 18:51:03.955967</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="n">
+        <v>599</v>
+      </c>
+      <c r="B600" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D600" t="inlineStr">
+        <is>
+          <t>2024-09-11 18:51:28.641593</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="n">
+        <v>600</v>
+      </c>
+      <c r="B601" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D601" t="inlineStr">
+        <is>
+          <t>2024-09-11 20:33:11.023739</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="n">
+        <v>601</v>
+      </c>
+      <c r="B602" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D602" t="inlineStr">
+        <is>
+          <t>2024-09-12 11:27:51.714233</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="n">
+        <v>602</v>
+      </c>
+      <c r="B603" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D603" t="inlineStr">
+        <is>
+          <t>2024-09-12 11:28:16.247171</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="n">
+        <v>603</v>
+      </c>
+      <c r="B604" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D604" t="inlineStr">
+        <is>
+          <t>2024-09-12 13:22:44.527374</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="n">
+        <v>604</v>
+      </c>
+      <c r="B605" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D605" t="inlineStr">
+        <is>
+          <t>2024-09-12 13:23:07.471917</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="n">
+        <v>605</v>
+      </c>
+      <c r="B606" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D606" t="inlineStr">
+        <is>
+          <t>2024-09-12 16:23:06.957921</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="n">
+        <v>606</v>
+      </c>
+      <c r="B607" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D607" t="inlineStr">
+        <is>
+          <t>2024-09-12 16:23:31.155864</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="n">
+        <v>607</v>
+      </c>
+      <c r="B608" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D608" t="inlineStr">
+        <is>
+          <t>2024-09-12 18:04:51.504088</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="n">
+        <v>608</v>
+      </c>
+      <c r="B609" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D609" t="inlineStr">
+        <is>
+          <t>2024-09-12 19:30:54.746527</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="n">
+        <v>609</v>
+      </c>
+      <c r="B610" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D610" t="inlineStr">
+        <is>
+          <t>2024-09-12 19:33:59.417788</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="n">
+        <v>610</v>
+      </c>
+      <c r="B611" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D611" t="inlineStr">
+        <is>
+          <t>2024-09-12 20:32:06.863036</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="n">
+        <v>611</v>
+      </c>
+      <c r="B612" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D612" t="inlineStr">
+        <is>
+          <t>2024-09-13 17:04:34.673992</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="n">
+        <v>612</v>
+      </c>
+      <c r="B613" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D613" t="inlineStr">
+        <is>
+          <t>2024-09-13 17:04:55.422607</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="n">
+        <v>613</v>
+      </c>
+      <c r="B614" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D614" t="inlineStr">
+        <is>
+          <t>2024-09-13 18:03:57.207681</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="n">
+        <v>614</v>
+      </c>
+      <c r="B615" t="n">
+        <v>961922211</v>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>2024-09-13 18:32:57.480427</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="n">
+        <v>615</v>
+      </c>
+      <c r="B616" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>2024-09-13 20:33:17.625748</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="n">
+        <v>616</v>
+      </c>
+      <c r="B617" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D617" t="inlineStr">
+        <is>
+          <t>2024-09-14 18:04:10.977455</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="n">
+        <v>617</v>
+      </c>
+      <c r="B618" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D618" t="inlineStr">
+        <is>
+          <t>2024-09-14 20:31:40.928767</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="n">
+        <v>618</v>
+      </c>
+      <c r="B619" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D619" t="inlineStr">
+        <is>
+          <t>2024-09-17 14:55:57.304475</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="n">
+        <v>619</v>
+      </c>
+      <c r="B620" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D620" t="inlineStr">
+        <is>
+          <t>2024-09-17 14:56:43.680920</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="n">
+        <v>620</v>
+      </c>
+      <c r="B621" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D621" t="inlineStr">
+        <is>
+          <t>2024-09-17 17:13:12.358995</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="n">
+        <v>621</v>
+      </c>
+      <c r="B622" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D622" t="inlineStr">
+        <is>
+          <t>2024-09-17 17:13:34.778023</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="n">
+        <v>622</v>
+      </c>
+      <c r="B623" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>Mengupdate laporan TS P2TL Sesuai Jadwal</t>
+        </is>
+      </c>
+      <c r="D623" t="inlineStr">
+        <is>
+          <t>2024-09-17 18:04:24.314804</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="n">
+        <v>623</v>
+      </c>
+      <c r="B624" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>mengupdate Realisasi H-1 P1 dan PD</t>
+        </is>
+      </c>
+      <c r="D624" t="inlineStr">
+        <is>
+          <t>2024-09-17 20:32:07.160647</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="n">
+        <v>624</v>
+      </c>
+      <c r="B625" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D625" t="inlineStr">
+        <is>
+          <t>2024-09-18 13:37:24.938830</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="n">
+        <v>625</v>
+      </c>
+      <c r="B626" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D626" t="inlineStr">
+        <is>
+          <t>2024-09-18 13:38:11.859671</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="n">
+        <v>626</v>
+      </c>
+      <c r="B627" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>Update Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D627" t="inlineStr">
+        <is>
+          <t>2024-09-18 15:42:19.801790</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="n">
+        <v>627</v>
+      </c>
+      <c r="B628" t="n">
+        <v>-4146843555</v>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>Kirim Laporan TS Harian</t>
+        </is>
+      </c>
+      <c r="D628" t="inlineStr">
+        <is>
+          <t>2024-09-18 15:57:46.885947</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>